<commit_message>
For each Excel Resolvido
</commit_message>
<xml_diff>
--- a/Criação do Sourcing-Performer/Data/Output/Planilha_Controle.xlsx
+++ b/Criação do Sourcing-Performer/Data/Output/Planilha_Controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProcurumentGarage 2\Criação do Sourcing-Performer\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE20A140-64A2-491D-87C6-F9797DFA96CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A3C97A-9B0E-447B-B6C8-896C4DDCD210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Requisição</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>TUBOS EM ACO CARBONO EM GERAL (CC SC...)</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,8 +441,8 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -455,13 +458,13 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3514</v>
+        <v>3515</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -472,25 +475,8 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3514</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste temporal nas atividades de Type Into/Click + adição de comentários
</commit_message>
<xml_diff>
--- a/Criação do Sourcing-Performer/Data/Output/Planilha_Controle.xlsx
+++ b/Criação do Sourcing-Performer/Data/Output/Planilha_Controle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProcurumentGarage 2\Criação do Sourcing-Performer\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68447EE3-EC5D-4B17-A3D9-96278201D636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2E651-F6AA-4B32-B3AC-CF93E6BA95B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="4560" windowWidth="15945" windowHeight="6975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3703</v>
+        <v>3606</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>

</xml_diff>